<commit_message>
Fix issues with oLCA flows that do not follow the reference unit, e.g., water flows in kg instead of m3.
</commit_message>
<xml_diff>
--- a/Data/mappings/oLCA/oLCA_mapping.xlsx
+++ b/Data/mappings/oLCA/oLCA_mapping.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\oLCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75586091-3C16-4816-99A9-346577EBD593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B480ABD4-D175-42D2-99C4-E2DE99CB4DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14105" uniqueCount="8403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14110" uniqueCount="8403">
   <si>
     <t>Theophylline</t>
   </si>
@@ -25656,9 +25656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8022"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -47897,6 +47895,9 @@
       <c r="A3157" s="1" t="s">
         <v>5461</v>
       </c>
+      <c r="B3157" s="1" t="s">
+        <v>4988</v>
+      </c>
     </row>
     <row r="3158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3158" s="1" t="s">
@@ -47948,6 +47949,9 @@
       <c r="A3166" s="1" t="s">
         <v>6541</v>
       </c>
+      <c r="B3166" s="1" t="s">
+        <v>4988</v>
+      </c>
     </row>
     <row r="3167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3167" s="1" t="s">
@@ -72234,6 +72238,9 @@
       <c r="A6510" s="1" t="s">
         <v>7418</v>
       </c>
+      <c r="B6510" s="1" t="s">
+        <v>5931</v>
+      </c>
     </row>
     <row r="6511" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6511" s="1" t="s">
@@ -74378,6 +74385,9 @@
       <c r="A6781" s="1" t="s">
         <v>7437</v>
       </c>
+      <c r="B6781" s="1" t="s">
+        <v>4763</v>
+      </c>
     </row>
     <row r="6782" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6782" s="1" t="s">
@@ -80583,6 +80593,9 @@
     <row r="7565" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7565" s="1" t="s">
         <v>7718</v>
+      </c>
+      <c r="B7565" s="1" t="s">
+        <v>4763</v>
       </c>
     </row>
     <row r="7566" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Few mapping corrections for openLCA. Still the whole water flows story to check.
</commit_message>
<xml_diff>
--- a/Data/mappings/oLCA/oLCA_mapping.xlsx
+++ b/Data/mappings/oLCA/oLCA_mapping.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\oLCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B480ABD4-D175-42D2-99C4-E2DE99CB4DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B1A94A-DE8D-43B3-B1FB-5E8CA65C8DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14110" uniqueCount="8403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14120" uniqueCount="8404">
   <si>
     <t>Theophylline</t>
   </si>
@@ -25241,6 +25241,9 @@
   </si>
   <si>
     <t>Water, well, in ground, ZW</t>
+  </si>
+  <si>
+    <t>Transformation, from secondary vegetation</t>
   </si>
 </sst>
 </file>
@@ -25656,7 +25659,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8022"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4453" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4481" sqref="B4481"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -41428,6 +41433,9 @@
       <c r="A2253" s="1" t="s">
         <v>6369</v>
       </c>
+      <c r="B2253" s="1" t="s">
+        <v>5759</v>
+      </c>
     </row>
     <row r="2254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2254" s="1" t="s">
@@ -41824,6 +41832,9 @@
       <c r="A2307" s="1" t="s">
         <v>4641</v>
       </c>
+      <c r="B2307" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="2308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2308" s="1" t="s">
@@ -50089,7 +50100,7 @@
         <v>4178</v>
       </c>
       <c r="B3490" s="1" t="s">
-        <v>2676</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="3491" spans="1:2" x14ac:dyDescent="0.3">
@@ -52218,6 +52229,9 @@
       <c r="A3784" s="1" t="s">
         <v>6720</v>
       </c>
+      <c r="B3784" s="1" t="s">
+        <v>2456</v>
+      </c>
     </row>
     <row r="3785" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3785" s="1" t="s">
@@ -52231,6 +52245,9 @@
       <c r="A3786" s="1" t="s">
         <v>6721</v>
       </c>
+      <c r="B3786" s="1" t="s">
+        <v>8098</v>
+      </c>
     </row>
     <row r="3787" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3787" s="1" t="s">
@@ -55408,6 +55425,9 @@
       <c r="A4215" s="1" t="s">
         <v>6777</v>
       </c>
+      <c r="B4215" s="1" t="s">
+        <v>2962</v>
+      </c>
     </row>
     <row r="4216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4216" s="1" t="s">
@@ -57317,11 +57337,17 @@
       <c r="A4472" s="1" t="s">
         <v>1939</v>
       </c>
+      <c r="B4472" s="1" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="4473" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4473" s="1" t="s">
         <v>6902</v>
       </c>
+      <c r="B4473" s="1" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="4474" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4474" s="1" t="s">
@@ -61450,16 +61476,25 @@
       <c r="A5061" s="1" t="s">
         <v>6996</v>
       </c>
+      <c r="B5061" s="1" t="s">
+        <v>2951</v>
+      </c>
     </row>
     <row r="5062" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5062" s="1" t="s">
         <v>6997</v>
       </c>
+      <c r="B5062" s="1" t="s">
+        <v>2951</v>
+      </c>
     </row>
     <row r="5063" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5063" s="1" t="s">
         <v>6998</v>
       </c>
+      <c r="B5063" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="5064" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5064" s="1" t="s">
@@ -65745,7 +65780,7 @@
         <v>7213</v>
       </c>
       <c r="B5663" s="1" t="s">
-        <v>8141</v>
+        <v>8403</v>
       </c>
     </row>
     <row r="5664" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Mapping errors for water turbine use flows corrected.
</commit_message>
<xml_diff>
--- a/Data/mappings/oLCA/oLCA_mapping.xlsx
+++ b/Data/mappings/oLCA/oLCA_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\oLCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B1A94A-DE8D-43B3-B1FB-5E8CA65C8DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3D9B30-9B0F-40A9-8756-13C5BE8FEBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14120" uniqueCount="8404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14120" uniqueCount="8398">
   <si>
     <t>Theophylline</t>
   </si>
@@ -24476,24 +24476,6 @@
   </si>
   <si>
     <t>Transformation, to permanent crops</t>
-  </si>
-  <si>
-    <t>Water, unspecified natural origin,BA</t>
-  </si>
-  <si>
-    <t>Water, unspecified natural origin, WT</t>
-  </si>
-  <si>
-    <t>Water, unspecified natural origin, lC</t>
-  </si>
-  <si>
-    <t>Water, unspecified natural origin. NI</t>
-  </si>
-  <si>
-    <t>Water, unspecified natural origin. NO</t>
-  </si>
-  <si>
-    <t>Water, unspecified natural origin TR</t>
   </si>
   <si>
     <t>Water, well, in ground, AD</t>
@@ -25659,8 +25641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8022"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4453" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4481" sqref="B4481"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40122,7 +40104,7 @@
         <v>5233</v>
       </c>
       <c r="B2068" s="1" t="s">
-        <v>5233</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="2069" spans="1:2" x14ac:dyDescent="0.3">
@@ -65780,7 +65762,7 @@
         <v>7213</v>
       </c>
       <c r="B5663" s="1" t="s">
-        <v>8403</v>
+        <v>8397</v>
       </c>
     </row>
     <row r="5664" spans="1:2" x14ac:dyDescent="0.3">
@@ -76627,7 +76609,7 @@
         <v>7464</v>
       </c>
       <c r="B7059" s="1" t="s">
-        <v>8148</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="7060" spans="1:2" x14ac:dyDescent="0.3">
@@ -77019,7 +77001,7 @@
         <v>7513</v>
       </c>
       <c r="B7108" s="1" t="s">
-        <v>8149</v>
+        <v>5258</v>
       </c>
     </row>
     <row r="7109" spans="1:2" x14ac:dyDescent="0.3">
@@ -77496,7 +77478,7 @@
         <v>7573</v>
       </c>
       <c r="B7168" s="1" t="s">
-        <v>8150</v>
+        <v>4664</v>
       </c>
     </row>
     <row r="7169" spans="1:2" x14ac:dyDescent="0.3">
@@ -77784,7 +77766,7 @@
         <v>7609</v>
       </c>
       <c r="B7204" s="1" t="s">
-        <v>8151</v>
+        <v>4801</v>
       </c>
     </row>
     <row r="7205" spans="1:2" x14ac:dyDescent="0.3">
@@ -77800,7 +77782,7 @@
         <v>7611</v>
       </c>
       <c r="B7206" s="1" t="s">
-        <v>8152</v>
+        <v>5594</v>
       </c>
     </row>
     <row r="7207" spans="1:2" x14ac:dyDescent="0.3">
@@ -78320,7 +78302,7 @@
         <v>7676</v>
       </c>
       <c r="B7271" s="1" t="s">
-        <v>8153</v>
+        <v>4221</v>
       </c>
     </row>
     <row r="7272" spans="1:2" x14ac:dyDescent="0.3">
@@ -80654,7 +80636,7 @@
         <v>7721</v>
       </c>
       <c r="B7568" s="1" t="s">
-        <v>8154</v>
+        <v>8148</v>
       </c>
     </row>
     <row r="7569" spans="1:2" x14ac:dyDescent="0.3">
@@ -80662,7 +80644,7 @@
         <v>7722</v>
       </c>
       <c r="B7569" s="1" t="s">
-        <v>8155</v>
+        <v>8149</v>
       </c>
     </row>
     <row r="7570" spans="1:2" x14ac:dyDescent="0.3">
@@ -80670,7 +80652,7 @@
         <v>7723</v>
       </c>
       <c r="B7570" s="1" t="s">
-        <v>8156</v>
+        <v>8150</v>
       </c>
     </row>
     <row r="7571" spans="1:2" x14ac:dyDescent="0.3">
@@ -80678,7 +80660,7 @@
         <v>7724</v>
       </c>
       <c r="B7571" s="1" t="s">
-        <v>8157</v>
+        <v>8151</v>
       </c>
     </row>
     <row r="7572" spans="1:2" x14ac:dyDescent="0.3">
@@ -80686,7 +80668,7 @@
         <v>7725</v>
       </c>
       <c r="B7572" s="1" t="s">
-        <v>8158</v>
+        <v>8152</v>
       </c>
     </row>
     <row r="7573" spans="1:2" x14ac:dyDescent="0.3">
@@ -80694,7 +80676,7 @@
         <v>7726</v>
       </c>
       <c r="B7573" s="1" t="s">
-        <v>8159</v>
+        <v>8153</v>
       </c>
     </row>
     <row r="7574" spans="1:2" x14ac:dyDescent="0.3">
@@ -80702,7 +80684,7 @@
         <v>7727</v>
       </c>
       <c r="B7574" s="1" t="s">
-        <v>8160</v>
+        <v>8154</v>
       </c>
     </row>
     <row r="7575" spans="1:2" x14ac:dyDescent="0.3">
@@ -80710,7 +80692,7 @@
         <v>7728</v>
       </c>
       <c r="B7575" s="1" t="s">
-        <v>8161</v>
+        <v>8155</v>
       </c>
     </row>
     <row r="7576" spans="1:2" x14ac:dyDescent="0.3">
@@ -80718,7 +80700,7 @@
         <v>7729</v>
       </c>
       <c r="B7576" s="1" t="s">
-        <v>8162</v>
+        <v>8156</v>
       </c>
     </row>
     <row r="7577" spans="1:2" x14ac:dyDescent="0.3">
@@ -80726,7 +80708,7 @@
         <v>7730</v>
       </c>
       <c r="B7577" s="1" t="s">
-        <v>8163</v>
+        <v>8157</v>
       </c>
     </row>
     <row r="7578" spans="1:2" x14ac:dyDescent="0.3">
@@ -80734,7 +80716,7 @@
         <v>7731</v>
       </c>
       <c r="B7578" s="1" t="s">
-        <v>8164</v>
+        <v>8158</v>
       </c>
     </row>
     <row r="7579" spans="1:2" x14ac:dyDescent="0.3">
@@ -80742,7 +80724,7 @@
         <v>7732</v>
       </c>
       <c r="B7579" s="1" t="s">
-        <v>8165</v>
+        <v>8159</v>
       </c>
     </row>
     <row r="7580" spans="1:2" x14ac:dyDescent="0.3">
@@ -80750,7 +80732,7 @@
         <v>7733</v>
       </c>
       <c r="B7580" s="1" t="s">
-        <v>8166</v>
+        <v>8160</v>
       </c>
     </row>
     <row r="7581" spans="1:2" x14ac:dyDescent="0.3">
@@ -80758,7 +80740,7 @@
         <v>7734</v>
       </c>
       <c r="B7581" s="1" t="s">
-        <v>8167</v>
+        <v>8161</v>
       </c>
     </row>
     <row r="7582" spans="1:2" x14ac:dyDescent="0.3">
@@ -80766,7 +80748,7 @@
         <v>7735</v>
       </c>
       <c r="B7582" s="1" t="s">
-        <v>8168</v>
+        <v>8162</v>
       </c>
     </row>
     <row r="7583" spans="1:2" x14ac:dyDescent="0.3">
@@ -80774,7 +80756,7 @@
         <v>7736</v>
       </c>
       <c r="B7583" s="1" t="s">
-        <v>8169</v>
+        <v>8163</v>
       </c>
     </row>
     <row r="7584" spans="1:2" x14ac:dyDescent="0.3">
@@ -80782,7 +80764,7 @@
         <v>7737</v>
       </c>
       <c r="B7584" s="1" t="s">
-        <v>8170</v>
+        <v>8164</v>
       </c>
     </row>
     <row r="7585" spans="1:2" x14ac:dyDescent="0.3">
@@ -80790,7 +80772,7 @@
         <v>7738</v>
       </c>
       <c r="B7585" s="1" t="s">
-        <v>8171</v>
+        <v>8165</v>
       </c>
     </row>
     <row r="7586" spans="1:2" x14ac:dyDescent="0.3">
@@ -80798,7 +80780,7 @@
         <v>7739</v>
       </c>
       <c r="B7586" s="1" t="s">
-        <v>8172</v>
+        <v>8166</v>
       </c>
     </row>
     <row r="7587" spans="1:2" x14ac:dyDescent="0.3">
@@ -80806,7 +80788,7 @@
         <v>7740</v>
       </c>
       <c r="B7587" s="1" t="s">
-        <v>8173</v>
+        <v>8167</v>
       </c>
     </row>
     <row r="7588" spans="1:2" x14ac:dyDescent="0.3">
@@ -80814,7 +80796,7 @@
         <v>7741</v>
       </c>
       <c r="B7588" s="1" t="s">
-        <v>8174</v>
+        <v>8168</v>
       </c>
     </row>
     <row r="7589" spans="1:2" x14ac:dyDescent="0.3">
@@ -80822,7 +80804,7 @@
         <v>7742</v>
       </c>
       <c r="B7589" s="1" t="s">
-        <v>8175</v>
+        <v>8169</v>
       </c>
     </row>
     <row r="7590" spans="1:2" x14ac:dyDescent="0.3">
@@ -80830,7 +80812,7 @@
         <v>7743</v>
       </c>
       <c r="B7590" s="1" t="s">
-        <v>8176</v>
+        <v>8170</v>
       </c>
     </row>
     <row r="7591" spans="1:2" x14ac:dyDescent="0.3">
@@ -80838,7 +80820,7 @@
         <v>7744</v>
       </c>
       <c r="B7591" s="1" t="s">
-        <v>8177</v>
+        <v>8171</v>
       </c>
     </row>
     <row r="7592" spans="1:2" x14ac:dyDescent="0.3">
@@ -80846,7 +80828,7 @@
         <v>7745</v>
       </c>
       <c r="B7592" s="1" t="s">
-        <v>8178</v>
+        <v>8172</v>
       </c>
     </row>
     <row r="7593" spans="1:2" x14ac:dyDescent="0.3">
@@ -80854,7 +80836,7 @@
         <v>7746</v>
       </c>
       <c r="B7593" s="1" t="s">
-        <v>8179</v>
+        <v>8173</v>
       </c>
     </row>
     <row r="7594" spans="1:2" x14ac:dyDescent="0.3">
@@ -80862,7 +80844,7 @@
         <v>7747</v>
       </c>
       <c r="B7594" s="1" t="s">
-        <v>8180</v>
+        <v>8174</v>
       </c>
     </row>
     <row r="7595" spans="1:2" x14ac:dyDescent="0.3">
@@ -80870,7 +80852,7 @@
         <v>7748</v>
       </c>
       <c r="B7595" s="1" t="s">
-        <v>8181</v>
+        <v>8175</v>
       </c>
     </row>
     <row r="7596" spans="1:2" x14ac:dyDescent="0.3">
@@ -80878,7 +80860,7 @@
         <v>7749</v>
       </c>
       <c r="B7596" s="1" t="s">
-        <v>8182</v>
+        <v>8176</v>
       </c>
     </row>
     <row r="7597" spans="1:2" x14ac:dyDescent="0.3">
@@ -80886,7 +80868,7 @@
         <v>7750</v>
       </c>
       <c r="B7597" s="1" t="s">
-        <v>8183</v>
+        <v>8177</v>
       </c>
     </row>
     <row r="7598" spans="1:2" x14ac:dyDescent="0.3">
@@ -80894,7 +80876,7 @@
         <v>7751</v>
       </c>
       <c r="B7598" s="1" t="s">
-        <v>8184</v>
+        <v>8178</v>
       </c>
     </row>
     <row r="7599" spans="1:2" x14ac:dyDescent="0.3">
@@ -80902,7 +80884,7 @@
         <v>7752</v>
       </c>
       <c r="B7599" s="1" t="s">
-        <v>8185</v>
+        <v>8179</v>
       </c>
     </row>
     <row r="7600" spans="1:2" x14ac:dyDescent="0.3">
@@ -80910,7 +80892,7 @@
         <v>7753</v>
       </c>
       <c r="B7600" s="1" t="s">
-        <v>8186</v>
+        <v>8180</v>
       </c>
     </row>
     <row r="7601" spans="1:2" x14ac:dyDescent="0.3">
@@ -80918,7 +80900,7 @@
         <v>7754</v>
       </c>
       <c r="B7601" s="1" t="s">
-        <v>8187</v>
+        <v>8181</v>
       </c>
     </row>
     <row r="7602" spans="1:2" x14ac:dyDescent="0.3">
@@ -80926,7 +80908,7 @@
         <v>7755</v>
       </c>
       <c r="B7602" s="1" t="s">
-        <v>8188</v>
+        <v>8182</v>
       </c>
     </row>
     <row r="7603" spans="1:2" x14ac:dyDescent="0.3">
@@ -80934,7 +80916,7 @@
         <v>7756</v>
       </c>
       <c r="B7603" s="1" t="s">
-        <v>8189</v>
+        <v>8183</v>
       </c>
     </row>
     <row r="7604" spans="1:2" x14ac:dyDescent="0.3">
@@ -80942,7 +80924,7 @@
         <v>7757</v>
       </c>
       <c r="B7604" s="1" t="s">
-        <v>8190</v>
+        <v>8184</v>
       </c>
     </row>
     <row r="7605" spans="1:2" x14ac:dyDescent="0.3">
@@ -80950,7 +80932,7 @@
         <v>7758</v>
       </c>
       <c r="B7605" s="1" t="s">
-        <v>8191</v>
+        <v>8185</v>
       </c>
     </row>
     <row r="7606" spans="1:2" x14ac:dyDescent="0.3">
@@ -80958,7 +80940,7 @@
         <v>7759</v>
       </c>
       <c r="B7606" s="1" t="s">
-        <v>8192</v>
+        <v>8186</v>
       </c>
     </row>
     <row r="7607" spans="1:2" x14ac:dyDescent="0.3">
@@ -80966,7 +80948,7 @@
         <v>7760</v>
       </c>
       <c r="B7607" s="1" t="s">
-        <v>8193</v>
+        <v>8187</v>
       </c>
     </row>
     <row r="7608" spans="1:2" x14ac:dyDescent="0.3">
@@ -80974,7 +80956,7 @@
         <v>7761</v>
       </c>
       <c r="B7608" s="1" t="s">
-        <v>8194</v>
+        <v>8188</v>
       </c>
     </row>
     <row r="7609" spans="1:2" x14ac:dyDescent="0.3">
@@ -80982,7 +80964,7 @@
         <v>7762</v>
       </c>
       <c r="B7609" s="1" t="s">
-        <v>8195</v>
+        <v>8189</v>
       </c>
     </row>
     <row r="7610" spans="1:2" x14ac:dyDescent="0.3">
@@ -80990,7 +80972,7 @@
         <v>7763</v>
       </c>
       <c r="B7610" s="1" t="s">
-        <v>8196</v>
+        <v>8190</v>
       </c>
     </row>
     <row r="7611" spans="1:2" x14ac:dyDescent="0.3">
@@ -80998,7 +80980,7 @@
         <v>7764</v>
       </c>
       <c r="B7611" s="1" t="s">
-        <v>8197</v>
+        <v>8191</v>
       </c>
     </row>
     <row r="7612" spans="1:2" x14ac:dyDescent="0.3">
@@ -81006,7 +80988,7 @@
         <v>7765</v>
       </c>
       <c r="B7612" s="1" t="s">
-        <v>8198</v>
+        <v>8192</v>
       </c>
     </row>
     <row r="7613" spans="1:2" x14ac:dyDescent="0.3">
@@ -81014,7 +80996,7 @@
         <v>7766</v>
       </c>
       <c r="B7613" s="1" t="s">
-        <v>8199</v>
+        <v>8193</v>
       </c>
     </row>
     <row r="7614" spans="1:2" x14ac:dyDescent="0.3">
@@ -81022,7 +81004,7 @@
         <v>7767</v>
       </c>
       <c r="B7614" s="1" t="s">
-        <v>8200</v>
+        <v>8194</v>
       </c>
     </row>
     <row r="7615" spans="1:2" x14ac:dyDescent="0.3">
@@ -81030,7 +81012,7 @@
         <v>7768</v>
       </c>
       <c r="B7615" s="1" t="s">
-        <v>8201</v>
+        <v>8195</v>
       </c>
     </row>
     <row r="7616" spans="1:2" x14ac:dyDescent="0.3">
@@ -81038,7 +81020,7 @@
         <v>7769</v>
       </c>
       <c r="B7616" s="1" t="s">
-        <v>8202</v>
+        <v>8196</v>
       </c>
     </row>
     <row r="7617" spans="1:2" x14ac:dyDescent="0.3">
@@ -81046,7 +81028,7 @@
         <v>7770</v>
       </c>
       <c r="B7617" s="1" t="s">
-        <v>8203</v>
+        <v>8197</v>
       </c>
     </row>
     <row r="7618" spans="1:2" x14ac:dyDescent="0.3">
@@ -81054,7 +81036,7 @@
         <v>7771</v>
       </c>
       <c r="B7618" s="1" t="s">
-        <v>8204</v>
+        <v>8198</v>
       </c>
     </row>
     <row r="7619" spans="1:2" x14ac:dyDescent="0.3">
@@ -81062,7 +81044,7 @@
         <v>7772</v>
       </c>
       <c r="B7619" s="1" t="s">
-        <v>8205</v>
+        <v>8199</v>
       </c>
     </row>
     <row r="7620" spans="1:2" x14ac:dyDescent="0.3">
@@ -81070,7 +81052,7 @@
         <v>7773</v>
       </c>
       <c r="B7620" s="1" t="s">
-        <v>8206</v>
+        <v>8200</v>
       </c>
     </row>
     <row r="7621" spans="1:2" x14ac:dyDescent="0.3">
@@ -81078,7 +81060,7 @@
         <v>7774</v>
       </c>
       <c r="B7621" s="1" t="s">
-        <v>8207</v>
+        <v>8201</v>
       </c>
     </row>
     <row r="7622" spans="1:2" x14ac:dyDescent="0.3">
@@ -81086,7 +81068,7 @@
         <v>7775</v>
       </c>
       <c r="B7622" s="1" t="s">
-        <v>8208</v>
+        <v>8202</v>
       </c>
     </row>
     <row r="7623" spans="1:2" x14ac:dyDescent="0.3">
@@ -81094,7 +81076,7 @@
         <v>7776</v>
       </c>
       <c r="B7623" s="1" t="s">
-        <v>8209</v>
+        <v>8203</v>
       </c>
     </row>
     <row r="7624" spans="1:2" x14ac:dyDescent="0.3">
@@ -81102,7 +81084,7 @@
         <v>7777</v>
       </c>
       <c r="B7624" s="1" t="s">
-        <v>8210</v>
+        <v>8204</v>
       </c>
     </row>
     <row r="7625" spans="1:2" x14ac:dyDescent="0.3">
@@ -81110,7 +81092,7 @@
         <v>7778</v>
       </c>
       <c r="B7625" s="1" t="s">
-        <v>8211</v>
+        <v>8205</v>
       </c>
     </row>
     <row r="7626" spans="1:2" x14ac:dyDescent="0.3">
@@ -81118,7 +81100,7 @@
         <v>7779</v>
       </c>
       <c r="B7626" s="1" t="s">
-        <v>8212</v>
+        <v>8206</v>
       </c>
     </row>
     <row r="7627" spans="1:2" x14ac:dyDescent="0.3">
@@ -81126,7 +81108,7 @@
         <v>7780</v>
       </c>
       <c r="B7627" s="1" t="s">
-        <v>8213</v>
+        <v>8207</v>
       </c>
     </row>
     <row r="7628" spans="1:2" x14ac:dyDescent="0.3">
@@ -81134,7 +81116,7 @@
         <v>7781</v>
       </c>
       <c r="B7628" s="1" t="s">
-        <v>8214</v>
+        <v>8208</v>
       </c>
     </row>
     <row r="7629" spans="1:2" x14ac:dyDescent="0.3">
@@ -81142,7 +81124,7 @@
         <v>7782</v>
       </c>
       <c r="B7629" s="1" t="s">
-        <v>8215</v>
+        <v>8209</v>
       </c>
     </row>
     <row r="7630" spans="1:2" x14ac:dyDescent="0.3">
@@ -81150,7 +81132,7 @@
         <v>7783</v>
       </c>
       <c r="B7630" s="1" t="s">
-        <v>8216</v>
+        <v>8210</v>
       </c>
     </row>
     <row r="7631" spans="1:2" x14ac:dyDescent="0.3">
@@ -81158,7 +81140,7 @@
         <v>7784</v>
       </c>
       <c r="B7631" s="1" t="s">
-        <v>8217</v>
+        <v>8211</v>
       </c>
     </row>
     <row r="7632" spans="1:2" x14ac:dyDescent="0.3">
@@ -81166,7 +81148,7 @@
         <v>7785</v>
       </c>
       <c r="B7632" s="1" t="s">
-        <v>8338</v>
+        <v>8332</v>
       </c>
     </row>
     <row r="7633" spans="1:2" x14ac:dyDescent="0.3">
@@ -81174,7 +81156,7 @@
         <v>7786</v>
       </c>
       <c r="B7633" s="1" t="s">
-        <v>8338</v>
+        <v>8332</v>
       </c>
     </row>
     <row r="7634" spans="1:2" x14ac:dyDescent="0.3">
@@ -81182,7 +81164,7 @@
         <v>7787</v>
       </c>
       <c r="B7634" s="1" t="s">
-        <v>8218</v>
+        <v>8212</v>
       </c>
     </row>
     <row r="7635" spans="1:2" x14ac:dyDescent="0.3">
@@ -81190,7 +81172,7 @@
         <v>7788</v>
       </c>
       <c r="B7635" s="1" t="s">
-        <v>8219</v>
+        <v>8213</v>
       </c>
     </row>
     <row r="7636" spans="1:2" x14ac:dyDescent="0.3">
@@ -81198,7 +81180,7 @@
         <v>7789</v>
       </c>
       <c r="B7636" s="1" t="s">
-        <v>8220</v>
+        <v>8214</v>
       </c>
     </row>
     <row r="7637" spans="1:2" x14ac:dyDescent="0.3">
@@ -81206,7 +81188,7 @@
         <v>7790</v>
       </c>
       <c r="B7637" s="1" t="s">
-        <v>8221</v>
+        <v>8215</v>
       </c>
     </row>
     <row r="7638" spans="1:2" x14ac:dyDescent="0.3">
@@ -81214,7 +81196,7 @@
         <v>7791</v>
       </c>
       <c r="B7638" s="1" t="s">
-        <v>8222</v>
+        <v>8216</v>
       </c>
     </row>
     <row r="7639" spans="1:2" x14ac:dyDescent="0.3">
@@ -81222,7 +81204,7 @@
         <v>7792</v>
       </c>
       <c r="B7639" s="1" t="s">
-        <v>8223</v>
+        <v>8217</v>
       </c>
     </row>
     <row r="7640" spans="1:2" x14ac:dyDescent="0.3">
@@ -81230,7 +81212,7 @@
         <v>7793</v>
       </c>
       <c r="B7640" s="1" t="s">
-        <v>8224</v>
+        <v>8218</v>
       </c>
     </row>
     <row r="7641" spans="1:2" x14ac:dyDescent="0.3">
@@ -81238,7 +81220,7 @@
         <v>7794</v>
       </c>
       <c r="B7641" s="1" t="s">
-        <v>8225</v>
+        <v>8219</v>
       </c>
     </row>
     <row r="7642" spans="1:2" x14ac:dyDescent="0.3">
@@ -81246,7 +81228,7 @@
         <v>7795</v>
       </c>
       <c r="B7642" s="1" t="s">
-        <v>8226</v>
+        <v>8220</v>
       </c>
     </row>
     <row r="7643" spans="1:2" x14ac:dyDescent="0.3">
@@ -81254,7 +81236,7 @@
         <v>7796</v>
       </c>
       <c r="B7643" s="1" t="s">
-        <v>8227</v>
+        <v>8221</v>
       </c>
     </row>
     <row r="7644" spans="1:2" x14ac:dyDescent="0.3">
@@ -81262,7 +81244,7 @@
         <v>7797</v>
       </c>
       <c r="B7644" s="1" t="s">
-        <v>8228</v>
+        <v>8222</v>
       </c>
     </row>
     <row r="7645" spans="1:2" x14ac:dyDescent="0.3">
@@ -81270,7 +81252,7 @@
         <v>7798</v>
       </c>
       <c r="B7645" s="1" t="s">
-        <v>8229</v>
+        <v>8223</v>
       </c>
     </row>
     <row r="7646" spans="1:2" x14ac:dyDescent="0.3">
@@ -81278,7 +81260,7 @@
         <v>7799</v>
       </c>
       <c r="B7646" s="1" t="s">
-        <v>8230</v>
+        <v>8224</v>
       </c>
     </row>
     <row r="7647" spans="1:2" x14ac:dyDescent="0.3">
@@ -81286,7 +81268,7 @@
         <v>7800</v>
       </c>
       <c r="B7647" s="1" t="s">
-        <v>8231</v>
+        <v>8225</v>
       </c>
     </row>
     <row r="7648" spans="1:2" x14ac:dyDescent="0.3">
@@ -81294,7 +81276,7 @@
         <v>7801</v>
       </c>
       <c r="B7648" s="1" t="s">
-        <v>8232</v>
+        <v>8226</v>
       </c>
     </row>
     <row r="7649" spans="1:2" x14ac:dyDescent="0.3">
@@ -81302,7 +81284,7 @@
         <v>7802</v>
       </c>
       <c r="B7649" s="1" t="s">
-        <v>8233</v>
+        <v>8227</v>
       </c>
     </row>
     <row r="7650" spans="1:2" x14ac:dyDescent="0.3">
@@ -81310,7 +81292,7 @@
         <v>7803</v>
       </c>
       <c r="B7650" s="1" t="s">
-        <v>8234</v>
+        <v>8228</v>
       </c>
     </row>
     <row r="7651" spans="1:2" x14ac:dyDescent="0.3">
@@ -81318,7 +81300,7 @@
         <v>7804</v>
       </c>
       <c r="B7651" s="1" t="s">
-        <v>8235</v>
+        <v>8229</v>
       </c>
     </row>
     <row r="7652" spans="1:2" x14ac:dyDescent="0.3">
@@ -81326,7 +81308,7 @@
         <v>7805</v>
       </c>
       <c r="B7652" s="1" t="s">
-        <v>8236</v>
+        <v>8230</v>
       </c>
     </row>
     <row r="7653" spans="1:2" x14ac:dyDescent="0.3">
@@ -81334,7 +81316,7 @@
         <v>7806</v>
       </c>
       <c r="B7653" s="1" t="s">
-        <v>8237</v>
+        <v>8231</v>
       </c>
     </row>
     <row r="7654" spans="1:2" x14ac:dyDescent="0.3">
@@ -81342,7 +81324,7 @@
         <v>7807</v>
       </c>
       <c r="B7654" s="1" t="s">
-        <v>8238</v>
+        <v>8232</v>
       </c>
     </row>
     <row r="7655" spans="1:2" x14ac:dyDescent="0.3">
@@ -81350,7 +81332,7 @@
         <v>7808</v>
       </c>
       <c r="B7655" s="1" t="s">
-        <v>8239</v>
+        <v>8233</v>
       </c>
     </row>
     <row r="7656" spans="1:2" x14ac:dyDescent="0.3">
@@ -81358,7 +81340,7 @@
         <v>7809</v>
       </c>
       <c r="B7656" s="1" t="s">
-        <v>8240</v>
+        <v>8234</v>
       </c>
     </row>
     <row r="7657" spans="1:2" x14ac:dyDescent="0.3">
@@ -81366,7 +81348,7 @@
         <v>7810</v>
       </c>
       <c r="B7657" s="1" t="s">
-        <v>8241</v>
+        <v>8235</v>
       </c>
     </row>
     <row r="7658" spans="1:2" x14ac:dyDescent="0.3">
@@ -81374,7 +81356,7 @@
         <v>7811</v>
       </c>
       <c r="B7658" s="1" t="s">
-        <v>8242</v>
+        <v>8236</v>
       </c>
     </row>
     <row r="7659" spans="1:2" x14ac:dyDescent="0.3">
@@ -81382,7 +81364,7 @@
         <v>7812</v>
       </c>
       <c r="B7659" s="1" t="s">
-        <v>8243</v>
+        <v>8237</v>
       </c>
     </row>
     <row r="7660" spans="1:2" x14ac:dyDescent="0.3">
@@ -81395,7 +81377,7 @@
         <v>7814</v>
       </c>
       <c r="B7661" s="1" t="s">
-        <v>8244</v>
+        <v>8238</v>
       </c>
     </row>
     <row r="7662" spans="1:2" x14ac:dyDescent="0.3">
@@ -81403,7 +81385,7 @@
         <v>7815</v>
       </c>
       <c r="B7662" s="1" t="s">
-        <v>8245</v>
+        <v>8239</v>
       </c>
     </row>
     <row r="7663" spans="1:2" x14ac:dyDescent="0.3">
@@ -81411,7 +81393,7 @@
         <v>7816</v>
       </c>
       <c r="B7663" s="1" t="s">
-        <v>8246</v>
+        <v>8240</v>
       </c>
     </row>
     <row r="7664" spans="1:2" x14ac:dyDescent="0.3">
@@ -81419,7 +81401,7 @@
         <v>7817</v>
       </c>
       <c r="B7664" s="1" t="s">
-        <v>8247</v>
+        <v>8241</v>
       </c>
     </row>
     <row r="7665" spans="1:2" x14ac:dyDescent="0.3">
@@ -81427,7 +81409,7 @@
         <v>7818</v>
       </c>
       <c r="B7665" s="1" t="s">
-        <v>8248</v>
+        <v>8242</v>
       </c>
     </row>
     <row r="7666" spans="1:2" x14ac:dyDescent="0.3">
@@ -81435,7 +81417,7 @@
         <v>7819</v>
       </c>
       <c r="B7666" s="1" t="s">
-        <v>8249</v>
+        <v>8243</v>
       </c>
     </row>
     <row r="7667" spans="1:2" x14ac:dyDescent="0.3">
@@ -81443,7 +81425,7 @@
         <v>7820</v>
       </c>
       <c r="B7667" s="1" t="s">
-        <v>8250</v>
+        <v>8244</v>
       </c>
     </row>
     <row r="7668" spans="1:2" x14ac:dyDescent="0.3">
@@ -81451,7 +81433,7 @@
         <v>7821</v>
       </c>
       <c r="B7668" s="1" t="s">
-        <v>8251</v>
+        <v>8245</v>
       </c>
     </row>
     <row r="7669" spans="1:2" x14ac:dyDescent="0.3">
@@ -81459,7 +81441,7 @@
         <v>7822</v>
       </c>
       <c r="B7669" s="1" t="s">
-        <v>8252</v>
+        <v>8246</v>
       </c>
     </row>
     <row r="7670" spans="1:2" x14ac:dyDescent="0.3">
@@ -81467,7 +81449,7 @@
         <v>7823</v>
       </c>
       <c r="B7670" s="1" t="s">
-        <v>8253</v>
+        <v>8247</v>
       </c>
     </row>
     <row r="7671" spans="1:2" x14ac:dyDescent="0.3">
@@ -81475,7 +81457,7 @@
         <v>7824</v>
       </c>
       <c r="B7671" s="1" t="s">
-        <v>8254</v>
+        <v>8248</v>
       </c>
     </row>
     <row r="7672" spans="1:2" x14ac:dyDescent="0.3">
@@ -81483,7 +81465,7 @@
         <v>7825</v>
       </c>
       <c r="B7672" s="1" t="s">
-        <v>8255</v>
+        <v>8249</v>
       </c>
     </row>
     <row r="7673" spans="1:2" x14ac:dyDescent="0.3">
@@ -81491,7 +81473,7 @@
         <v>7826</v>
       </c>
       <c r="B7673" s="1" t="s">
-        <v>8256</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="7674" spans="1:2" x14ac:dyDescent="0.3">
@@ -81499,7 +81481,7 @@
         <v>7827</v>
       </c>
       <c r="B7674" s="1" t="s">
-        <v>8257</v>
+        <v>8251</v>
       </c>
     </row>
     <row r="7675" spans="1:2" x14ac:dyDescent="0.3">
@@ -81507,7 +81489,7 @@
         <v>7828</v>
       </c>
       <c r="B7675" s="1" t="s">
-        <v>8258</v>
+        <v>8252</v>
       </c>
     </row>
     <row r="7676" spans="1:2" x14ac:dyDescent="0.3">
@@ -81515,7 +81497,7 @@
         <v>7829</v>
       </c>
       <c r="B7676" s="1" t="s">
-        <v>8259</v>
+        <v>8253</v>
       </c>
     </row>
     <row r="7677" spans="1:2" x14ac:dyDescent="0.3">
@@ -81523,7 +81505,7 @@
         <v>7830</v>
       </c>
       <c r="B7677" s="1" t="s">
-        <v>8260</v>
+        <v>8254</v>
       </c>
     </row>
     <row r="7678" spans="1:2" x14ac:dyDescent="0.3">
@@ -81531,7 +81513,7 @@
         <v>7831</v>
       </c>
       <c r="B7678" s="1" t="s">
-        <v>8261</v>
+        <v>8255</v>
       </c>
     </row>
     <row r="7679" spans="1:2" x14ac:dyDescent="0.3">
@@ -81539,7 +81521,7 @@
         <v>7832</v>
       </c>
       <c r="B7679" s="1" t="s">
-        <v>8262</v>
+        <v>8256</v>
       </c>
     </row>
     <row r="7680" spans="1:2" x14ac:dyDescent="0.3">
@@ -81547,7 +81529,7 @@
         <v>7833</v>
       </c>
       <c r="B7680" s="1" t="s">
-        <v>8263</v>
+        <v>8257</v>
       </c>
     </row>
     <row r="7681" spans="1:2" x14ac:dyDescent="0.3">
@@ -81555,7 +81537,7 @@
         <v>7834</v>
       </c>
       <c r="B7681" s="1" t="s">
-        <v>8264</v>
+        <v>8258</v>
       </c>
     </row>
     <row r="7682" spans="1:2" x14ac:dyDescent="0.3">
@@ -81563,7 +81545,7 @@
         <v>7835</v>
       </c>
       <c r="B7682" s="1" t="s">
-        <v>8265</v>
+        <v>8259</v>
       </c>
     </row>
     <row r="7683" spans="1:2" x14ac:dyDescent="0.3">
@@ -81571,7 +81553,7 @@
         <v>7836</v>
       </c>
       <c r="B7683" s="1" t="s">
-        <v>8266</v>
+        <v>8260</v>
       </c>
     </row>
     <row r="7684" spans="1:2" x14ac:dyDescent="0.3">
@@ -81579,7 +81561,7 @@
         <v>7837</v>
       </c>
       <c r="B7684" s="1" t="s">
-        <v>8267</v>
+        <v>8261</v>
       </c>
     </row>
     <row r="7685" spans="1:2" x14ac:dyDescent="0.3">
@@ -81587,7 +81569,7 @@
         <v>7838</v>
       </c>
       <c r="B7685" s="1" t="s">
-        <v>8268</v>
+        <v>8262</v>
       </c>
     </row>
     <row r="7686" spans="1:2" x14ac:dyDescent="0.3">
@@ -81595,7 +81577,7 @@
         <v>7839</v>
       </c>
       <c r="B7686" s="1" t="s">
-        <v>8269</v>
+        <v>8263</v>
       </c>
     </row>
     <row r="7687" spans="1:2" x14ac:dyDescent="0.3">
@@ -81603,7 +81585,7 @@
         <v>7840</v>
       </c>
       <c r="B7687" s="1" t="s">
-        <v>8270</v>
+        <v>8264</v>
       </c>
     </row>
     <row r="7688" spans="1:2" x14ac:dyDescent="0.3">
@@ -81611,7 +81593,7 @@
         <v>7841</v>
       </c>
       <c r="B7688" s="1" t="s">
-        <v>8271</v>
+        <v>8265</v>
       </c>
     </row>
     <row r="7689" spans="1:2" x14ac:dyDescent="0.3">
@@ -81619,7 +81601,7 @@
         <v>7842</v>
       </c>
       <c r="B7689" s="1" t="s">
-        <v>8272</v>
+        <v>8266</v>
       </c>
     </row>
     <row r="7690" spans="1:2" x14ac:dyDescent="0.3">
@@ -81627,7 +81609,7 @@
         <v>7843</v>
       </c>
       <c r="B7690" s="1" t="s">
-        <v>8273</v>
+        <v>8267</v>
       </c>
     </row>
     <row r="7691" spans="1:2" x14ac:dyDescent="0.3">
@@ -81635,7 +81617,7 @@
         <v>7844</v>
       </c>
       <c r="B7691" s="1" t="s">
-        <v>8274</v>
+        <v>8268</v>
       </c>
     </row>
     <row r="7692" spans="1:2" x14ac:dyDescent="0.3">
@@ -81643,7 +81625,7 @@
         <v>7845</v>
       </c>
       <c r="B7692" s="1" t="s">
-        <v>8275</v>
+        <v>8269</v>
       </c>
     </row>
     <row r="7693" spans="1:2" x14ac:dyDescent="0.3">
@@ -81651,7 +81633,7 @@
         <v>7846</v>
       </c>
       <c r="B7693" s="1" t="s">
-        <v>8276</v>
+        <v>8270</v>
       </c>
     </row>
     <row r="7694" spans="1:2" x14ac:dyDescent="0.3">
@@ -81659,7 +81641,7 @@
         <v>7847</v>
       </c>
       <c r="B7694" s="1" t="s">
-        <v>8277</v>
+        <v>8271</v>
       </c>
     </row>
     <row r="7695" spans="1:2" x14ac:dyDescent="0.3">
@@ -81667,7 +81649,7 @@
         <v>7848</v>
       </c>
       <c r="B7695" s="1" t="s">
-        <v>8278</v>
+        <v>8272</v>
       </c>
     </row>
     <row r="7696" spans="1:2" x14ac:dyDescent="0.3">
@@ -81675,7 +81657,7 @@
         <v>7849</v>
       </c>
       <c r="B7696" s="1" t="s">
-        <v>8279</v>
+        <v>8273</v>
       </c>
     </row>
     <row r="7697" spans="1:2" x14ac:dyDescent="0.3">
@@ -81683,7 +81665,7 @@
         <v>7850</v>
       </c>
       <c r="B7697" s="1" t="s">
-        <v>8280</v>
+        <v>8274</v>
       </c>
     </row>
     <row r="7698" spans="1:2" x14ac:dyDescent="0.3">
@@ -81691,7 +81673,7 @@
         <v>7851</v>
       </c>
       <c r="B7698" s="1" t="s">
-        <v>8281</v>
+        <v>8275</v>
       </c>
     </row>
     <row r="7699" spans="1:2" x14ac:dyDescent="0.3">
@@ -81699,7 +81681,7 @@
         <v>7852</v>
       </c>
       <c r="B7699" s="1" t="s">
-        <v>8282</v>
+        <v>8276</v>
       </c>
     </row>
     <row r="7700" spans="1:2" x14ac:dyDescent="0.3">
@@ -81707,7 +81689,7 @@
         <v>7853</v>
       </c>
       <c r="B7700" s="1" t="s">
-        <v>8283</v>
+        <v>8277</v>
       </c>
     </row>
     <row r="7701" spans="1:2" x14ac:dyDescent="0.3">
@@ -81715,7 +81697,7 @@
         <v>7854</v>
       </c>
       <c r="B7701" s="1" t="s">
-        <v>8284</v>
+        <v>8278</v>
       </c>
     </row>
     <row r="7702" spans="1:2" x14ac:dyDescent="0.3">
@@ -81723,7 +81705,7 @@
         <v>7855</v>
       </c>
       <c r="B7702" s="1" t="s">
-        <v>8285</v>
+        <v>8279</v>
       </c>
     </row>
     <row r="7703" spans="1:2" x14ac:dyDescent="0.3">
@@ -81731,7 +81713,7 @@
         <v>7856</v>
       </c>
       <c r="B7703" s="1" t="s">
-        <v>8286</v>
+        <v>8280</v>
       </c>
     </row>
     <row r="7704" spans="1:2" x14ac:dyDescent="0.3">
@@ -81739,7 +81721,7 @@
         <v>7857</v>
       </c>
       <c r="B7704" s="1" t="s">
-        <v>8287</v>
+        <v>8281</v>
       </c>
     </row>
     <row r="7705" spans="1:2" x14ac:dyDescent="0.3">
@@ -81747,7 +81729,7 @@
         <v>7858</v>
       </c>
       <c r="B7705" s="1" t="s">
-        <v>8288</v>
+        <v>8282</v>
       </c>
     </row>
     <row r="7706" spans="1:2" x14ac:dyDescent="0.3">
@@ -81755,7 +81737,7 @@
         <v>7859</v>
       </c>
       <c r="B7706" s="1" t="s">
-        <v>8289</v>
+        <v>8283</v>
       </c>
     </row>
     <row r="7707" spans="1:2" x14ac:dyDescent="0.3">
@@ -81763,7 +81745,7 @@
         <v>7860</v>
       </c>
       <c r="B7707" s="1" t="s">
-        <v>8290</v>
+        <v>8284</v>
       </c>
     </row>
     <row r="7708" spans="1:2" x14ac:dyDescent="0.3">
@@ -81771,7 +81753,7 @@
         <v>7861</v>
       </c>
       <c r="B7708" s="1" t="s">
-        <v>8291</v>
+        <v>8285</v>
       </c>
     </row>
     <row r="7709" spans="1:2" x14ac:dyDescent="0.3">
@@ -81779,7 +81761,7 @@
         <v>7862</v>
       </c>
       <c r="B7709" s="1" t="s">
-        <v>8292</v>
+        <v>8286</v>
       </c>
     </row>
     <row r="7710" spans="1:2" x14ac:dyDescent="0.3">
@@ -81787,7 +81769,7 @@
         <v>7863</v>
       </c>
       <c r="B7710" s="1" t="s">
-        <v>8293</v>
+        <v>8287</v>
       </c>
     </row>
     <row r="7711" spans="1:2" x14ac:dyDescent="0.3">
@@ -81795,7 +81777,7 @@
         <v>7864</v>
       </c>
       <c r="B7711" s="1" t="s">
-        <v>8294</v>
+        <v>8288</v>
       </c>
     </row>
     <row r="7712" spans="1:2" x14ac:dyDescent="0.3">
@@ -81803,7 +81785,7 @@
         <v>7865</v>
       </c>
       <c r="B7712" s="1" t="s">
-        <v>8295</v>
+        <v>8289</v>
       </c>
     </row>
     <row r="7713" spans="1:2" x14ac:dyDescent="0.3">
@@ -81811,7 +81793,7 @@
         <v>7866</v>
       </c>
       <c r="B7713" s="1" t="s">
-        <v>8296</v>
+        <v>8290</v>
       </c>
     </row>
     <row r="7714" spans="1:2" x14ac:dyDescent="0.3">
@@ -81819,7 +81801,7 @@
         <v>7867</v>
       </c>
       <c r="B7714" s="1" t="s">
-        <v>8297</v>
+        <v>8291</v>
       </c>
     </row>
     <row r="7715" spans="1:2" x14ac:dyDescent="0.3">
@@ -81827,7 +81809,7 @@
         <v>7868</v>
       </c>
       <c r="B7715" s="1" t="s">
-        <v>8298</v>
+        <v>8292</v>
       </c>
     </row>
     <row r="7716" spans="1:2" x14ac:dyDescent="0.3">
@@ -81835,7 +81817,7 @@
         <v>7869</v>
       </c>
       <c r="B7716" s="1" t="s">
-        <v>8299</v>
+        <v>8293</v>
       </c>
     </row>
     <row r="7717" spans="1:2" x14ac:dyDescent="0.3">
@@ -81843,7 +81825,7 @@
         <v>7870</v>
       </c>
       <c r="B7717" s="1" t="s">
-        <v>8300</v>
+        <v>8294</v>
       </c>
     </row>
     <row r="7718" spans="1:2" x14ac:dyDescent="0.3">
@@ -81851,7 +81833,7 @@
         <v>7871</v>
       </c>
       <c r="B7718" s="1" t="s">
-        <v>8301</v>
+        <v>8295</v>
       </c>
     </row>
     <row r="7719" spans="1:2" x14ac:dyDescent="0.3">
@@ -81859,7 +81841,7 @@
         <v>7872</v>
       </c>
       <c r="B7719" s="1" t="s">
-        <v>8302</v>
+        <v>8296</v>
       </c>
     </row>
     <row r="7720" spans="1:2" x14ac:dyDescent="0.3">
@@ -81867,7 +81849,7 @@
         <v>7873</v>
       </c>
       <c r="B7720" s="1" t="s">
-        <v>8303</v>
+        <v>8297</v>
       </c>
     </row>
     <row r="7721" spans="1:2" x14ac:dyDescent="0.3">
@@ -81875,7 +81857,7 @@
         <v>7874</v>
       </c>
       <c r="B7721" s="1" t="s">
-        <v>8304</v>
+        <v>8298</v>
       </c>
     </row>
     <row r="7722" spans="1:2" x14ac:dyDescent="0.3">
@@ -81883,7 +81865,7 @@
         <v>7875</v>
       </c>
       <c r="B7722" s="1" t="s">
-        <v>8305</v>
+        <v>8299</v>
       </c>
     </row>
     <row r="7723" spans="1:2" x14ac:dyDescent="0.3">
@@ -81891,7 +81873,7 @@
         <v>7876</v>
       </c>
       <c r="B7723" s="1" t="s">
-        <v>8306</v>
+        <v>8300</v>
       </c>
     </row>
     <row r="7724" spans="1:2" x14ac:dyDescent="0.3">
@@ -81899,7 +81881,7 @@
         <v>7877</v>
       </c>
       <c r="B7724" s="1" t="s">
-        <v>8307</v>
+        <v>8301</v>
       </c>
     </row>
     <row r="7725" spans="1:2" x14ac:dyDescent="0.3">
@@ -81907,7 +81889,7 @@
         <v>7878</v>
       </c>
       <c r="B7725" s="1" t="s">
-        <v>8308</v>
+        <v>8302</v>
       </c>
     </row>
     <row r="7726" spans="1:2" x14ac:dyDescent="0.3">
@@ -81915,7 +81897,7 @@
         <v>7879</v>
       </c>
       <c r="B7726" s="1" t="s">
-        <v>8309</v>
+        <v>8303</v>
       </c>
     </row>
     <row r="7727" spans="1:2" x14ac:dyDescent="0.3">
@@ -81923,7 +81905,7 @@
         <v>7880</v>
       </c>
       <c r="B7727" s="1" t="s">
-        <v>8310</v>
+        <v>8304</v>
       </c>
     </row>
     <row r="7728" spans="1:2" x14ac:dyDescent="0.3">
@@ -81931,7 +81913,7 @@
         <v>7881</v>
       </c>
       <c r="B7728" s="1" t="s">
-        <v>8311</v>
+        <v>8305</v>
       </c>
     </row>
     <row r="7729" spans="1:2" x14ac:dyDescent="0.3">
@@ -81939,7 +81921,7 @@
         <v>7882</v>
       </c>
       <c r="B7729" s="1" t="s">
-        <v>8312</v>
+        <v>8306</v>
       </c>
     </row>
     <row r="7730" spans="1:2" x14ac:dyDescent="0.3">
@@ -81947,7 +81929,7 @@
         <v>7883</v>
       </c>
       <c r="B7730" s="1" t="s">
-        <v>8313</v>
+        <v>8307</v>
       </c>
     </row>
     <row r="7731" spans="1:2" x14ac:dyDescent="0.3">
@@ -81955,7 +81937,7 @@
         <v>7884</v>
       </c>
       <c r="B7731" s="1" t="s">
-        <v>8314</v>
+        <v>8308</v>
       </c>
     </row>
     <row r="7732" spans="1:2" x14ac:dyDescent="0.3">
@@ -81963,7 +81945,7 @@
         <v>7885</v>
       </c>
       <c r="B7732" s="1" t="s">
-        <v>8315</v>
+        <v>8309</v>
       </c>
     </row>
     <row r="7733" spans="1:2" x14ac:dyDescent="0.3">
@@ -81971,7 +81953,7 @@
         <v>7886</v>
       </c>
       <c r="B7733" s="1" t="s">
-        <v>8316</v>
+        <v>8310</v>
       </c>
     </row>
     <row r="7734" spans="1:2" x14ac:dyDescent="0.3">
@@ -81979,7 +81961,7 @@
         <v>7887</v>
       </c>
       <c r="B7734" s="1" t="s">
-        <v>8317</v>
+        <v>8311</v>
       </c>
     </row>
     <row r="7735" spans="1:2" x14ac:dyDescent="0.3">
@@ -81987,7 +81969,7 @@
         <v>7888</v>
       </c>
       <c r="B7735" s="1" t="s">
-        <v>8318</v>
+        <v>8312</v>
       </c>
     </row>
     <row r="7736" spans="1:2" x14ac:dyDescent="0.3">
@@ -81995,7 +81977,7 @@
         <v>7889</v>
       </c>
       <c r="B7736" s="1" t="s">
-        <v>8319</v>
+        <v>8313</v>
       </c>
     </row>
     <row r="7737" spans="1:2" x14ac:dyDescent="0.3">
@@ -82003,7 +81985,7 @@
         <v>7890</v>
       </c>
       <c r="B7737" s="1" t="s">
-        <v>8320</v>
+        <v>8314</v>
       </c>
     </row>
     <row r="7738" spans="1:2" x14ac:dyDescent="0.3">
@@ -82011,7 +81993,7 @@
         <v>7891</v>
       </c>
       <c r="B7738" s="1" t="s">
-        <v>8321</v>
+        <v>8315</v>
       </c>
     </row>
     <row r="7739" spans="1:2" x14ac:dyDescent="0.3">
@@ -82019,7 +82001,7 @@
         <v>7892</v>
       </c>
       <c r="B7739" s="1" t="s">
-        <v>8322</v>
+        <v>8316</v>
       </c>
     </row>
     <row r="7740" spans="1:2" x14ac:dyDescent="0.3">
@@ -82027,7 +82009,7 @@
         <v>7893</v>
       </c>
       <c r="B7740" s="1" t="s">
-        <v>8323</v>
+        <v>8317</v>
       </c>
     </row>
     <row r="7741" spans="1:2" x14ac:dyDescent="0.3">
@@ -82035,7 +82017,7 @@
         <v>7894</v>
       </c>
       <c r="B7741" s="1" t="s">
-        <v>8324</v>
+        <v>8318</v>
       </c>
     </row>
     <row r="7742" spans="1:2" x14ac:dyDescent="0.3">
@@ -82043,7 +82025,7 @@
         <v>7895</v>
       </c>
       <c r="B7742" s="1" t="s">
-        <v>8325</v>
+        <v>8319</v>
       </c>
     </row>
     <row r="7743" spans="1:2" x14ac:dyDescent="0.3">
@@ -82051,7 +82033,7 @@
         <v>7896</v>
       </c>
       <c r="B7743" s="1" t="s">
-        <v>8326</v>
+        <v>8320</v>
       </c>
     </row>
     <row r="7744" spans="1:2" x14ac:dyDescent="0.3">
@@ -82059,7 +82041,7 @@
         <v>7897</v>
       </c>
       <c r="B7744" s="1" t="s">
-        <v>8327</v>
+        <v>8321</v>
       </c>
     </row>
     <row r="7745" spans="1:2" x14ac:dyDescent="0.3">
@@ -82067,7 +82049,7 @@
         <v>7898</v>
       </c>
       <c r="B7745" s="1" t="s">
-        <v>8328</v>
+        <v>8322</v>
       </c>
     </row>
     <row r="7746" spans="1:2" x14ac:dyDescent="0.3">
@@ -82075,7 +82057,7 @@
         <v>7899</v>
       </c>
       <c r="B7746" s="1" t="s">
-        <v>8329</v>
+        <v>8323</v>
       </c>
     </row>
     <row r="7747" spans="1:2" x14ac:dyDescent="0.3">
@@ -82083,7 +82065,7 @@
         <v>7900</v>
       </c>
       <c r="B7747" s="1" t="s">
-        <v>8330</v>
+        <v>8324</v>
       </c>
     </row>
     <row r="7748" spans="1:2" x14ac:dyDescent="0.3">
@@ -82091,7 +82073,7 @@
         <v>7901</v>
       </c>
       <c r="B7748" s="1" t="s">
-        <v>8331</v>
+        <v>8325</v>
       </c>
     </row>
     <row r="7749" spans="1:2" x14ac:dyDescent="0.3">
@@ -82099,7 +82081,7 @@
         <v>7902</v>
       </c>
       <c r="B7749" s="1" t="s">
-        <v>8332</v>
+        <v>8326</v>
       </c>
     </row>
     <row r="7750" spans="1:2" x14ac:dyDescent="0.3">
@@ -82107,7 +82089,7 @@
         <v>7903</v>
       </c>
       <c r="B7750" s="1" t="s">
-        <v>8333</v>
+        <v>8327</v>
       </c>
     </row>
     <row r="7751" spans="1:2" x14ac:dyDescent="0.3">
@@ -82115,7 +82097,7 @@
         <v>7904</v>
       </c>
       <c r="B7751" s="1" t="s">
-        <v>8334</v>
+        <v>8328</v>
       </c>
     </row>
     <row r="7752" spans="1:2" x14ac:dyDescent="0.3">
@@ -82123,7 +82105,7 @@
         <v>7905</v>
       </c>
       <c r="B7752" s="1" t="s">
-        <v>8335</v>
+        <v>8329</v>
       </c>
     </row>
     <row r="7753" spans="1:2" x14ac:dyDescent="0.3">
@@ -82131,7 +82113,7 @@
         <v>7906</v>
       </c>
       <c r="B7753" s="1" t="s">
-        <v>8336</v>
+        <v>8330</v>
       </c>
     </row>
     <row r="7754" spans="1:2" x14ac:dyDescent="0.3">
@@ -82139,7 +82121,7 @@
         <v>7907</v>
       </c>
       <c r="B7754" s="1" t="s">
-        <v>8337</v>
+        <v>8331</v>
       </c>
     </row>
     <row r="7755" spans="1:2" x14ac:dyDescent="0.3">
@@ -82147,7 +82129,7 @@
         <v>7908</v>
       </c>
       <c r="B7755" s="1" t="s">
-        <v>8338</v>
+        <v>8332</v>
       </c>
     </row>
     <row r="7756" spans="1:2" x14ac:dyDescent="0.3">
@@ -82155,7 +82137,7 @@
         <v>7909</v>
       </c>
       <c r="B7756" s="1" t="s">
-        <v>8339</v>
+        <v>8333</v>
       </c>
     </row>
     <row r="7757" spans="1:2" x14ac:dyDescent="0.3">
@@ -82163,7 +82145,7 @@
         <v>7910</v>
       </c>
       <c r="B7757" s="1" t="s">
-        <v>8340</v>
+        <v>8334</v>
       </c>
     </row>
     <row r="7758" spans="1:2" x14ac:dyDescent="0.3">
@@ -82171,7 +82153,7 @@
         <v>7911</v>
       </c>
       <c r="B7758" s="1" t="s">
-        <v>8341</v>
+        <v>8335</v>
       </c>
     </row>
     <row r="7759" spans="1:2" x14ac:dyDescent="0.3">
@@ -82179,7 +82161,7 @@
         <v>7912</v>
       </c>
       <c r="B7759" s="1" t="s">
-        <v>8342</v>
+        <v>8336</v>
       </c>
     </row>
     <row r="7760" spans="1:2" x14ac:dyDescent="0.3">
@@ -82187,7 +82169,7 @@
         <v>7913</v>
       </c>
       <c r="B7760" s="1" t="s">
-        <v>8343</v>
+        <v>8337</v>
       </c>
     </row>
     <row r="7761" spans="1:2" x14ac:dyDescent="0.3">
@@ -82195,7 +82177,7 @@
         <v>7914</v>
       </c>
       <c r="B7761" s="1" t="s">
-        <v>8344</v>
+        <v>8338</v>
       </c>
     </row>
     <row r="7762" spans="1:2" x14ac:dyDescent="0.3">
@@ -82203,7 +82185,7 @@
         <v>7915</v>
       </c>
       <c r="B7762" s="1" t="s">
-        <v>8345</v>
+        <v>8339</v>
       </c>
     </row>
     <row r="7763" spans="1:2" x14ac:dyDescent="0.3">
@@ -82211,7 +82193,7 @@
         <v>7916</v>
       </c>
       <c r="B7763" s="1" t="s">
-        <v>8346</v>
+        <v>8340</v>
       </c>
     </row>
     <row r="7764" spans="1:2" x14ac:dyDescent="0.3">
@@ -82219,7 +82201,7 @@
         <v>7917</v>
       </c>
       <c r="B7764" s="1" t="s">
-        <v>8347</v>
+        <v>8341</v>
       </c>
     </row>
     <row r="7765" spans="1:2" x14ac:dyDescent="0.3">
@@ -82227,7 +82209,7 @@
         <v>7918</v>
       </c>
       <c r="B7765" s="1" t="s">
-        <v>8348</v>
+        <v>8342</v>
       </c>
     </row>
     <row r="7766" spans="1:2" x14ac:dyDescent="0.3">
@@ -82235,7 +82217,7 @@
         <v>7919</v>
       </c>
       <c r="B7766" s="1" t="s">
-        <v>8349</v>
+        <v>8343</v>
       </c>
     </row>
     <row r="7767" spans="1:2" x14ac:dyDescent="0.3">
@@ -82243,7 +82225,7 @@
         <v>7920</v>
       </c>
       <c r="B7767" s="1" t="s">
-        <v>8350</v>
+        <v>8344</v>
       </c>
     </row>
     <row r="7768" spans="1:2" x14ac:dyDescent="0.3">
@@ -82251,7 +82233,7 @@
         <v>7921</v>
       </c>
       <c r="B7768" s="1" t="s">
-        <v>8351</v>
+        <v>8345</v>
       </c>
     </row>
     <row r="7769" spans="1:2" x14ac:dyDescent="0.3">
@@ -82259,7 +82241,7 @@
         <v>7922</v>
       </c>
       <c r="B7769" s="1" t="s">
-        <v>8352</v>
+        <v>8346</v>
       </c>
     </row>
     <row r="7770" spans="1:2" x14ac:dyDescent="0.3">
@@ -82267,7 +82249,7 @@
         <v>7923</v>
       </c>
       <c r="B7770" s="1" t="s">
-        <v>8353</v>
+        <v>8347</v>
       </c>
     </row>
     <row r="7771" spans="1:2" x14ac:dyDescent="0.3">
@@ -82275,7 +82257,7 @@
         <v>7924</v>
       </c>
       <c r="B7771" s="1" t="s">
-        <v>8354</v>
+        <v>8348</v>
       </c>
     </row>
     <row r="7772" spans="1:2" x14ac:dyDescent="0.3">
@@ -82283,7 +82265,7 @@
         <v>7925</v>
       </c>
       <c r="B7772" s="1" t="s">
-        <v>8355</v>
+        <v>8349</v>
       </c>
     </row>
     <row r="7773" spans="1:2" x14ac:dyDescent="0.3">
@@ -82291,7 +82273,7 @@
         <v>7926</v>
       </c>
       <c r="B7773" s="1" t="s">
-        <v>8356</v>
+        <v>8350</v>
       </c>
     </row>
     <row r="7774" spans="1:2" x14ac:dyDescent="0.3">
@@ -82299,7 +82281,7 @@
         <v>7927</v>
       </c>
       <c r="B7774" s="1" t="s">
-        <v>8357</v>
+        <v>8351</v>
       </c>
     </row>
     <row r="7775" spans="1:2" x14ac:dyDescent="0.3">
@@ -82307,7 +82289,7 @@
         <v>7928</v>
       </c>
       <c r="B7775" s="1" t="s">
-        <v>8358</v>
+        <v>8352</v>
       </c>
     </row>
     <row r="7776" spans="1:2" x14ac:dyDescent="0.3">
@@ -82315,7 +82297,7 @@
         <v>7929</v>
       </c>
       <c r="B7776" s="1" t="s">
-        <v>8359</v>
+        <v>8353</v>
       </c>
     </row>
     <row r="7777" spans="1:2" x14ac:dyDescent="0.3">
@@ -82323,7 +82305,7 @@
         <v>7930</v>
       </c>
       <c r="B7777" s="1" t="s">
-        <v>8360</v>
+        <v>8354</v>
       </c>
     </row>
     <row r="7778" spans="1:2" x14ac:dyDescent="0.3">
@@ -82331,7 +82313,7 @@
         <v>7931</v>
       </c>
       <c r="B7778" s="1" t="s">
-        <v>8361</v>
+        <v>8355</v>
       </c>
     </row>
     <row r="7779" spans="1:2" x14ac:dyDescent="0.3">
@@ -82339,7 +82321,7 @@
         <v>7932</v>
       </c>
       <c r="B7779" s="1" t="s">
-        <v>8362</v>
+        <v>8356</v>
       </c>
     </row>
     <row r="7780" spans="1:2" x14ac:dyDescent="0.3">
@@ -82347,7 +82329,7 @@
         <v>7933</v>
       </c>
       <c r="B7780" s="1" t="s">
-        <v>8363</v>
+        <v>8357</v>
       </c>
     </row>
     <row r="7781" spans="1:2" x14ac:dyDescent="0.3">
@@ -82355,7 +82337,7 @@
         <v>7934</v>
       </c>
       <c r="B7781" s="1" t="s">
-        <v>8364</v>
+        <v>8358</v>
       </c>
     </row>
     <row r="7782" spans="1:2" x14ac:dyDescent="0.3">
@@ -82363,7 +82345,7 @@
         <v>7935</v>
       </c>
       <c r="B7782" s="1" t="s">
-        <v>8365</v>
+        <v>8359</v>
       </c>
     </row>
     <row r="7783" spans="1:2" x14ac:dyDescent="0.3">
@@ -82371,7 +82353,7 @@
         <v>7936</v>
       </c>
       <c r="B7783" s="1" t="s">
-        <v>8366</v>
+        <v>8360</v>
       </c>
     </row>
     <row r="7784" spans="1:2" x14ac:dyDescent="0.3">
@@ -82379,7 +82361,7 @@
         <v>7937</v>
       </c>
       <c r="B7784" s="1" t="s">
-        <v>8367</v>
+        <v>8361</v>
       </c>
     </row>
     <row r="7785" spans="1:2" x14ac:dyDescent="0.3">
@@ -82387,7 +82369,7 @@
         <v>7938</v>
       </c>
       <c r="B7785" s="1" t="s">
-        <v>8368</v>
+        <v>8362</v>
       </c>
     </row>
     <row r="7786" spans="1:2" x14ac:dyDescent="0.3">
@@ -82395,7 +82377,7 @@
         <v>7939</v>
       </c>
       <c r="B7786" s="1" t="s">
-        <v>8369</v>
+        <v>8363</v>
       </c>
     </row>
     <row r="7787" spans="1:2" x14ac:dyDescent="0.3">
@@ -82403,7 +82385,7 @@
         <v>7940</v>
       </c>
       <c r="B7787" s="1" t="s">
-        <v>8370</v>
+        <v>8364</v>
       </c>
     </row>
     <row r="7788" spans="1:2" x14ac:dyDescent="0.3">
@@ -82411,7 +82393,7 @@
         <v>7941</v>
       </c>
       <c r="B7788" s="1" t="s">
-        <v>8371</v>
+        <v>8365</v>
       </c>
     </row>
     <row r="7789" spans="1:2" x14ac:dyDescent="0.3">
@@ -82419,7 +82401,7 @@
         <v>7942</v>
       </c>
       <c r="B7789" s="1" t="s">
-        <v>8372</v>
+        <v>8366</v>
       </c>
     </row>
     <row r="7790" spans="1:2" x14ac:dyDescent="0.3">
@@ -82427,7 +82409,7 @@
         <v>7943</v>
       </c>
       <c r="B7790" s="1" t="s">
-        <v>8373</v>
+        <v>8367</v>
       </c>
     </row>
     <row r="7791" spans="1:2" x14ac:dyDescent="0.3">
@@ -82435,7 +82417,7 @@
         <v>7944</v>
       </c>
       <c r="B7791" s="1" t="s">
-        <v>8374</v>
+        <v>8368</v>
       </c>
     </row>
     <row r="7792" spans="1:2" x14ac:dyDescent="0.3">
@@ -82443,7 +82425,7 @@
         <v>7945</v>
       </c>
       <c r="B7792" s="1" t="s">
-        <v>8375</v>
+        <v>8369</v>
       </c>
     </row>
     <row r="7793" spans="1:2" x14ac:dyDescent="0.3">
@@ -82451,7 +82433,7 @@
         <v>7946</v>
       </c>
       <c r="B7793" s="1" t="s">
-        <v>8376</v>
+        <v>8370</v>
       </c>
     </row>
     <row r="7794" spans="1:2" x14ac:dyDescent="0.3">
@@ -82459,7 +82441,7 @@
         <v>7947</v>
       </c>
       <c r="B7794" s="1" t="s">
-        <v>8377</v>
+        <v>8371</v>
       </c>
     </row>
     <row r="7795" spans="1:2" x14ac:dyDescent="0.3">
@@ -82467,7 +82449,7 @@
         <v>7948</v>
       </c>
       <c r="B7795" s="1" t="s">
-        <v>8378</v>
+        <v>8372</v>
       </c>
     </row>
     <row r="7796" spans="1:2" x14ac:dyDescent="0.3">
@@ -82475,7 +82457,7 @@
         <v>7949</v>
       </c>
       <c r="B7796" s="1" t="s">
-        <v>8379</v>
+        <v>8373</v>
       </c>
     </row>
     <row r="7797" spans="1:2" x14ac:dyDescent="0.3">
@@ -82483,7 +82465,7 @@
         <v>7950</v>
       </c>
       <c r="B7797" s="1" t="s">
-        <v>8380</v>
+        <v>8374</v>
       </c>
     </row>
     <row r="7798" spans="1:2" x14ac:dyDescent="0.3">
@@ -82491,7 +82473,7 @@
         <v>7951</v>
       </c>
       <c r="B7798" s="1" t="s">
-        <v>8381</v>
+        <v>8375</v>
       </c>
     </row>
     <row r="7799" spans="1:2" x14ac:dyDescent="0.3">
@@ -82499,7 +82481,7 @@
         <v>7952</v>
       </c>
       <c r="B7799" s="1" t="s">
-        <v>8382</v>
+        <v>8376</v>
       </c>
     </row>
     <row r="7800" spans="1:2" x14ac:dyDescent="0.3">
@@ -82507,7 +82489,7 @@
         <v>7953</v>
       </c>
       <c r="B7800" s="1" t="s">
-        <v>8383</v>
+        <v>8377</v>
       </c>
     </row>
     <row r="7801" spans="1:2" x14ac:dyDescent="0.3">
@@ -82515,7 +82497,7 @@
         <v>7954</v>
       </c>
       <c r="B7801" s="1" t="s">
-        <v>8384</v>
+        <v>8378</v>
       </c>
     </row>
     <row r="7802" spans="1:2" x14ac:dyDescent="0.3">
@@ -82523,7 +82505,7 @@
         <v>7955</v>
       </c>
       <c r="B7802" s="1" t="s">
-        <v>8385</v>
+        <v>8379</v>
       </c>
     </row>
     <row r="7803" spans="1:2" x14ac:dyDescent="0.3">
@@ -82531,7 +82513,7 @@
         <v>7956</v>
       </c>
       <c r="B7803" s="1" t="s">
-        <v>8386</v>
+        <v>8380</v>
       </c>
     </row>
     <row r="7804" spans="1:2" x14ac:dyDescent="0.3">
@@ -82539,7 +82521,7 @@
         <v>7957</v>
       </c>
       <c r="B7804" s="1" t="s">
-        <v>8387</v>
+        <v>8381</v>
       </c>
     </row>
     <row r="7805" spans="1:2" x14ac:dyDescent="0.3">
@@ -82547,7 +82529,7 @@
         <v>7958</v>
       </c>
       <c r="B7805" s="1" t="s">
-        <v>8388</v>
+        <v>8382</v>
       </c>
     </row>
     <row r="7806" spans="1:2" x14ac:dyDescent="0.3">
@@ -82555,7 +82537,7 @@
         <v>7959</v>
       </c>
       <c r="B7806" s="1" t="s">
-        <v>8389</v>
+        <v>8383</v>
       </c>
     </row>
     <row r="7807" spans="1:2" x14ac:dyDescent="0.3">
@@ -82563,7 +82545,7 @@
         <v>7960</v>
       </c>
       <c r="B7807" s="1" t="s">
-        <v>8390</v>
+        <v>8384</v>
       </c>
     </row>
     <row r="7808" spans="1:2" x14ac:dyDescent="0.3">
@@ -82571,7 +82553,7 @@
         <v>7961</v>
       </c>
       <c r="B7808" s="1" t="s">
-        <v>8391</v>
+        <v>8385</v>
       </c>
     </row>
     <row r="7809" spans="1:2" x14ac:dyDescent="0.3">
@@ -82579,7 +82561,7 @@
         <v>7962</v>
       </c>
       <c r="B7809" s="1" t="s">
-        <v>8392</v>
+        <v>8386</v>
       </c>
     </row>
     <row r="7810" spans="1:2" x14ac:dyDescent="0.3">
@@ -82587,7 +82569,7 @@
         <v>7963</v>
       </c>
       <c r="B7810" s="1" t="s">
-        <v>8393</v>
+        <v>8387</v>
       </c>
     </row>
     <row r="7811" spans="1:2" x14ac:dyDescent="0.3">
@@ -82595,7 +82577,7 @@
         <v>7964</v>
       </c>
       <c r="B7811" s="1" t="s">
-        <v>8394</v>
+        <v>8388</v>
       </c>
     </row>
     <row r="7812" spans="1:2" x14ac:dyDescent="0.3">
@@ -82603,7 +82585,7 @@
         <v>7965</v>
       </c>
       <c r="B7812" s="1" t="s">
-        <v>8395</v>
+        <v>8389</v>
       </c>
     </row>
     <row r="7813" spans="1:2" x14ac:dyDescent="0.3">
@@ -82611,7 +82593,7 @@
         <v>7966</v>
       </c>
       <c r="B7813" s="1" t="s">
-        <v>8396</v>
+        <v>8390</v>
       </c>
     </row>
     <row r="7814" spans="1:2" x14ac:dyDescent="0.3">
@@ -82619,7 +82601,7 @@
         <v>7967</v>
       </c>
       <c r="B7814" s="1" t="s">
-        <v>8397</v>
+        <v>8391</v>
       </c>
     </row>
     <row r="7815" spans="1:2" x14ac:dyDescent="0.3">
@@ -82627,7 +82609,7 @@
         <v>7968</v>
       </c>
       <c r="B7815" s="1" t="s">
-        <v>8398</v>
+        <v>8392</v>
       </c>
     </row>
     <row r="7816" spans="1:2" x14ac:dyDescent="0.3">
@@ -82635,7 +82617,7 @@
         <v>7969</v>
       </c>
       <c r="B7816" s="1" t="s">
-        <v>8399</v>
+        <v>8393</v>
       </c>
     </row>
     <row r="7817" spans="1:2" x14ac:dyDescent="0.3">
@@ -82643,7 +82625,7 @@
         <v>7970</v>
       </c>
       <c r="B7817" s="1" t="s">
-        <v>8400</v>
+        <v>8394</v>
       </c>
     </row>
     <row r="7818" spans="1:2" x14ac:dyDescent="0.3">
@@ -82651,7 +82633,7 @@
         <v>7971</v>
       </c>
       <c r="B7818" s="1" t="s">
-        <v>8401</v>
+        <v>8395</v>
       </c>
     </row>
     <row r="7819" spans="1:2" x14ac:dyDescent="0.3">
@@ -82659,7 +82641,7 @@
         <v>7972</v>
       </c>
       <c r="B7819" s="1" t="s">
-        <v>8402</v>
+        <v>8396</v>
       </c>
     </row>
     <row r="7820" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>